<commit_message>
configs for case study 1 functional
</commit_message>
<xml_diff>
--- a/example/eO/data/xESM_1_inventory.xlsx
+++ b/example/eO/data/xESM_1_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desho/CORAL-eO/example/eO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAC4AD2-AB95-0743-BC3F-B385FFAB4EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B3F174-A328-2740-A09F-1FF080EF5500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="-17500" windowWidth="27760" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="27760" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>Item</t>
   </si>
@@ -67,15 +67,6 @@
   </si>
   <si>
     <t>Fridges - 5 needed</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>321</t>
@@ -1454,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1475,36 +1466,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1512,8 +1503,8 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
+      <c r="D2" s="6">
+        <v>1</v>
       </c>
       <c r="E2" s="6">
         <v>399.16</v>
@@ -1525,7 +1516,7 @@
     </row>
     <row r="3" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -1533,8 +1524,8 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
+      <c r="D3" s="6">
+        <v>1</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1544,7 +1535,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -1552,8 +1543,8 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
+      <c r="D4" s="6">
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <f>6*470*0.617</f>
@@ -1571,7 +1562,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>4</v>
@@ -1579,8 +1570,8 @@
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
+      <c r="D5" s="6">
+        <v>1</v>
       </c>
       <c r="E5" s="6">
         <f>E4*1.165</f>
@@ -1596,7 +1587,7 @@
     </row>
     <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -1604,20 +1595,20 @@
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -1625,7 +1616,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1633,8 +1624,8 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>14</v>
+      <c r="D7" s="7">
+        <v>1</v>
       </c>
       <c r="E7" s="7">
         <v>36.6</v>
@@ -1654,7 +1645,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>1</v>
@@ -1662,8 +1653,8 @@
       <c r="C8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>14</v>
+      <c r="D8" s="9">
+        <v>1</v>
       </c>
       <c r="E8" s="6">
         <v>399.16</v>
@@ -1681,7 +1672,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>1</v>
@@ -1689,8 +1680,8 @@
       <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
+      <c r="D9" s="9">
+        <v>1</v>
       </c>
       <c r="E9" s="9">
         <v>1665.9</v>
@@ -1706,7 +1697,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>4</v>
@@ -1714,8 +1705,8 @@
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
+      <c r="D10" s="9">
+        <v>1</v>
       </c>
       <c r="E10" s="9">
         <f>260*6*0.617</f>
@@ -1733,7 +1724,7 @@
     </row>
     <row r="11" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>4</v>
@@ -1741,8 +1732,8 @@
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
+      <c r="D11" s="9">
+        <v>1</v>
       </c>
       <c r="E11" s="9">
         <f>E10*1.165</f>
@@ -1760,7 +1751,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>4</v>
@@ -1768,20 +1759,20 @@
       <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
@@ -1789,7 +1780,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -1797,8 +1788,8 @@
       <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
+      <c r="D13" s="10">
+        <v>1</v>
       </c>
       <c r="E13" s="10">
         <v>36.6</v>
@@ -1818,7 +1809,7 @@
     </row>
     <row r="14" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>1</v>
@@ -1826,8 +1817,8 @@
       <c r="C14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>14</v>
+      <c r="D14" s="9">
+        <v>1</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1837,7 +1828,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>1</v>
@@ -1845,8 +1836,8 @@
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
+      <c r="D15" s="9">
+        <v>1</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1856,7 +1847,7 @@
     </row>
     <row r="16" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>4</v>
@@ -1864,8 +1855,8 @@
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>14</v>
+      <c r="D16" s="9">
+        <v>1</v>
       </c>
       <c r="E16" s="9">
         <f>210*6*0.617</f>
@@ -1883,7 +1874,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>4</v>
@@ -1891,8 +1882,8 @@
       <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
+      <c r="D17" s="9">
+        <v>1</v>
       </c>
       <c r="E17" s="9">
         <f>E16*1.165</f>
@@ -1908,7 +1899,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>4</v>
@@ -1916,20 +1907,20 @@
       <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="G18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="I18" s="9">
         <v>0</v>
@@ -1937,7 +1928,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
@@ -1945,8 +1936,8 @@
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>14</v>
+      <c r="D19" s="10">
+        <v>1</v>
       </c>
       <c r="E19" s="10">
         <v>36.6</v>

</xml_diff>